<commit_message>
Working on packaging of project.
</commit_message>
<xml_diff>
--- a/PatentDataOrganizer/testFile.xlsx
+++ b/PatentDataOrganizer/testFile.xlsx
@@ -26,34 +26,34 @@
     <t>Good</t>
   </si>
   <si>
+    <t>1341503</t>
+  </si>
+  <si>
     <t>2552925</t>
   </si>
   <si>
-    <t>1341518</t>
-  </si>
-  <si>
-    <t>2544843</t>
-  </si>
-  <si>
-    <t>1341517</t>
-  </si>
-  <si>
-    <t>2005311</t>
+    <t>2542254</t>
+  </si>
+  <si>
+    <t>2562856</t>
+  </si>
+  <si>
+    <t>2542261</t>
+  </si>
+  <si>
+    <t>2332066</t>
+  </si>
+  <si>
+    <t>2222015</t>
+  </si>
+  <si>
+    <t>1341496</t>
+  </si>
+  <si>
+    <t>2552920</t>
   </si>
   <si>
     <t>2562861</t>
-  </si>
-  <si>
-    <t>1341498</t>
-  </si>
-  <si>
-    <t>2008418</t>
-  </si>
-  <si>
-    <t>2545994</t>
-  </si>
-  <si>
-    <t>1341496</t>
   </si>
 </sst>
 </file>
@@ -114,10 +114,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.83984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="3.20703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.15625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.15625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="3.515625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.6875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>